<commit_message>
Added GUI and integration test cases to use case folder for A00a and A00b.
</commit_message>
<xml_diff>
--- a/Adventurer/Adv_UseCases/A00_InitQuit/QUIT_TestSummary.xlsx
+++ b/Adventurer/Adv_UseCases/A00_InitQuit/QUIT_TestSummary.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TA##_Aaaa" sheetId="1" r:id="rId1"/>
-    <sheet name="Reviewer Comments" sheetId="2" r:id="rId2"/>
+    <sheet name="GUI" sheetId="1" r:id="rId1"/>
+    <sheet name="Integration" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -79,21 +79,6 @@
     <t>Use Case:</t>
   </si>
   <si>
-    <t>Reviewer Comments</t>
-  </si>
-  <si>
-    <t>Reviewer</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>TA##_Aaaaa</t>
-  </si>
-  <si>
     <t>- Remember to update the tab name for the test case.</t>
   </si>
   <si>
@@ -158,19 +143,42 @@
   </si>
   <si>
     <t>Adventurer state is as when left, re: Hero and Building states; clock starts from where its previous value</t>
+  </si>
+  <si>
+    <t>non-HIC Object.Methods</t>
+  </si>
+  <si>
+    <t>GUI only</t>
+  </si>
+  <si>
+    <t>MainframeCiv.quit()
+Adventurer.approvedQuit()
+Adventurer.closeRegistries()</t>
+  </si>
+  <si>
+    <t>QUIT from menubar, window close event, or command line</t>
+  </si>
+  <si>
+    <t>QUIT from menubar, window Close event, or QUIT from command line</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -238,14 +246,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <u/>
       <sz val="12"/>
@@ -259,6 +259,53 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -305,89 +352,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -396,14 +436,49 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -433,57 +508,18 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:C31" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A4:C31"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Reviewer" dataDxfId="2"/>
-    <tableColumn id="2" name="Date" dataDxfId="1"/>
-    <tableColumn id="3" name="Comments" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -826,37 +862,37 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="40" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="21" customFormat="1" ht="30">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="16" customFormat="1" ht="30">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -876,11 +912,11 @@
         <v>1</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>38</v>
+      <c r="C5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -891,11 +927,11 @@
         <v>2</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>38</v>
+      <c r="C6" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -906,11 +942,11 @@
         <v>3</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>38</v>
+      <c r="C7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -921,11 +957,11 @@
         <v>4</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>31</v>
+      <c r="C8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -936,11 +972,11 @@
         <v>5</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>33</v>
+      <c r="C9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -951,11 +987,11 @@
         <v>6</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>35</v>
+      <c r="C10" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -966,11 +1002,11 @@
         <v>7</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>45</v>
+      <c r="C11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -981,11 +1017,11 @@
         <v>8</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>44</v>
+      <c r="C12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -996,8 +1032,8 @@
         <v>9</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1007,8 +1043,8 @@
         <v>10</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1016,8 +1052,8 @@
     <row r="15" spans="1:7">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1038,11 +1074,11 @@
         <v>1</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>42</v>
+      <c r="C17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1053,8 +1089,8 @@
         <v>2</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1064,8 +1100,8 @@
         <v>3</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="4"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1075,8 +1111,8 @@
         <v>4</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1086,8 +1122,8 @@
         <v>5</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1097,8 +1133,8 @@
         <v>6</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1215,10 +1251,10 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1321,12 +1357,12 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1342,184 +1378,479 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="18"/>
-    <col min="3" max="3" width="71.5" style="18" customWidth="1"/>
+    <col min="1" max="1" width="13" style="27" customWidth="1"/>
+    <col min="2" max="2" width="12" style="20" customWidth="1"/>
+    <col min="3" max="4" width="30" style="20" customWidth="1"/>
+    <col min="5" max="5" width="12" style="20" customWidth="1"/>
+    <col min="6" max="6" width="39" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="40" customHeight="1">
+      <c r="A2" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="30" customFormat="1" ht="30">
+      <c r="A3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" ht="43" customHeight="1">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="26">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="1:6" ht="39">
+      <c r="A8" s="3">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" ht="39">
+      <c r="A9" s="3">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="24"/>
+    </row>
+    <row r="10" spans="1:6" ht="52">
+      <c r="A10" s="3">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" ht="26">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="3">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="24"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="24"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="24"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="3">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="24"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="24"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="23"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="3">
+        <v>2</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="24"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="3">
+        <v>3</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="24"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="3">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="24"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="3"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="24"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8">
+        <f>COUNT(B5:B15)+COUNT(B17:B27)+COUNT(B29:B31)+COUNT(B33:B37)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="8">
+        <f>COUNT(C5:C15)+COUNT(C17:C27)+COUNT(C29:C31)+COUNT(C33:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8">
+        <f>COUNT(E5:E15)+COUNT(E17:E27)+COUNT(E29:E31)+COUNT(E33:E37)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="25"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="16" t="s">
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Slight changes while reviewing use cases and test cases.
</commit_message>
<xml_diff>
--- a/Adventurer/Adv_UseCases/A00_InitQuit/QUIT_TestSummary.xlsx
+++ b/Adventurer/Adv_UseCases/A00_InitQuit/QUIT_TestSummary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27440" windowHeight="17060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUI" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>QUIT from menubar, window Close event, or QUIT from command line</t>
+  </si>
+  <si>
+    <t>Adventurer state is as when left, re: Hero and Building states; clock starts from its previous value</t>
   </si>
 </sst>
 </file>
@@ -1380,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1511,7 +1514,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="1:6" ht="52">
+    <row r="10" spans="1:6" ht="39">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="24"/>

</xml_diff>